<commit_message>
LG bot 1 scraping and writing reports done with config file
</commit_message>
<xml_diff>
--- a/Scrape_Bot1/Data/Config.xlsx
+++ b/Scrape_Bot1/Data/Config.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RPA\RPA_WebScraping\Scrape_Bot1\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{961C5E95-6575-405E-B095-2725EFC7237A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28DFED39-0D9B-453C-BB08-CA93A43A69C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4332" yWindow="1560" windowWidth="17604" windowHeight="9936" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Settings" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Name</t>
   </si>
@@ -36,19 +36,13 @@
     <t>Manufacturer_Path</t>
   </si>
   <si>
-    <t>D:\MainExcel.xlsx</t>
-  </si>
-  <si>
-    <t>Start_URL</t>
-  </si>
-  <si>
-    <t>https://www.google.com/</t>
-  </si>
-  <si>
     <t>ReportPath</t>
   </si>
   <si>
     <t>D:\ReportsScraping\</t>
+  </si>
+  <si>
+    <t>Data\MasterULRs.xlsx</t>
   </si>
 </sst>
 </file>
@@ -375,10 +369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -400,23 +394,15 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new logic for comparision added to the code
</commit_message>
<xml_diff>
--- a/Scrape_Bot1/Data/Config.xlsx
+++ b/Scrape_Bot1/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RPA\RPA_WebScraping\Scrape_Bot1\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28DFED39-0D9B-453C-BB08-CA93A43A69C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AAC1048-3C58-4BD7-99BA-7B6A0A18CDC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Name</t>
   </si>
@@ -36,13 +36,19 @@
     <t>Manufacturer_Path</t>
   </si>
   <si>
-    <t>ReportPath</t>
-  </si>
-  <si>
-    <t>D:\ReportsScraping\</t>
-  </si>
-  <si>
     <t>Data\MasterULRs.xlsx</t>
+  </si>
+  <si>
+    <t>D:\ReportsScraping\Bot 1\</t>
+  </si>
+  <si>
+    <t>ReportPath_Bot1</t>
+  </si>
+  <si>
+    <t>ReportPath_main</t>
+  </si>
+  <si>
+    <t>D:\ReportsScraping\MAIN.xlsx</t>
   </si>
 </sst>
 </file>
@@ -369,10 +375,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -394,15 +400,23 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>